<commit_message>
fix data in xlsx
</commit_message>
<xml_diff>
--- a/GovtBonds+FPIs.xlsx
+++ b/GovtBonds+FPIs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Rouhin Projects\Nityoday. Geetha. I RP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\RG-GI-RP\FPI-bonds-relations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BF0E222-83CE-4CA6-BAD3-2B897EC050A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14921E37-ECF0-4C23-8FF1-B59181AABFB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="2" r:id="rId1"/>
@@ -1073,10 +1073,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P137"/>
+  <dimension ref="A1:P136"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5345,70 +5345,22 @@
       </c>
     </row>
     <row r="136" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A136" s="3" t="e">
-        <f ca="1">_xll.BDH(B130,B135:C135,B131,B132,"Dir=V","Dts=S","Sort=D","Quote=C","QtTyp=P","Days=T",CONCATENATE("Per=c",B133),"DtFmt=D","UseDPDF=Y","cols=3;rows=141")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="B136" s="4">
-        <v>113.79</v>
-      </c>
-      <c r="C136" s="4">
-        <v>6.8529999999999998</v>
-      </c>
-      <c r="D136" s="5">
-        <v>57724</v>
-      </c>
-      <c r="E136" s="5">
-        <v>1299</v>
-      </c>
-      <c r="F136" s="5">
-        <v>8592</v>
-      </c>
-      <c r="G136" s="5">
-        <v>22959</v>
-      </c>
-      <c r="H136" s="5">
-        <v>2455</v>
-      </c>
-      <c r="I136" s="5">
-        <v>-14</v>
-      </c>
-      <c r="J136" s="5">
-        <v>891</v>
-      </c>
-      <c r="K136" s="5">
-        <v>-8</v>
-      </c>
-      <c r="L136" s="5">
-        <v>0</v>
-      </c>
-      <c r="M136" s="5">
-        <v>-359</v>
-      </c>
-      <c r="N136" s="5">
-        <v>0</v>
-      </c>
-      <c r="O136" s="5">
-        <v>93538</v>
-      </c>
-    </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="D137" s="2"/>
-      <c r="E137" s="2"/>
-      <c r="F137" s="2"/>
-      <c r="G137" s="2"/>
-      <c r="H137" s="2"/>
-      <c r="I137" s="2"/>
-      <c r="J137" s="2"/>
-      <c r="K137" s="2"/>
-      <c r="L137" s="2"/>
-      <c r="M137" s="2"/>
-      <c r="N137" s="2"/>
-      <c r="O137" s="2"/>
+      <c r="D136" s="2"/>
+      <c r="E136" s="2"/>
+      <c r="F136" s="2"/>
+      <c r="G136" s="2"/>
+      <c r="H136" s="2"/>
+      <c r="I136" s="2"/>
+      <c r="J136" s="2"/>
+      <c r="K136" s="2"/>
+      <c r="L136" s="2"/>
+      <c r="M136" s="2"/>
+      <c r="N136" s="2"/>
+      <c r="O136" s="2"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:C136">
-    <sortCondition ref="A1:A136"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:C135">
+    <sortCondition ref="A1:A135"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>